<commit_message>
normalize version in sheets
</commit_message>
<xml_diff>
--- a/wheel_post_processing/packages_to_process_non_noarch-v2.xlsx
+++ b/wheel_post_processing/packages_to_process_non_noarch-v2.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$90</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="140">
   <si>
     <t xml:space="preserve">package_name</t>
   </si>
@@ -37,7 +40,7 @@
     <t xml:space="preserve">torch</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0.0a0+gite9ebda2</t>
+    <t xml:space="preserve">2.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">torch-2.0.0a0+gite9ebda2-cp310-cp310-linux_ppc64le.whl</t>
@@ -49,7 +52,7 @@
     <t xml:space="preserve">torch-2.0.0a0+gite9ebda2-cp39-cp39-linux_ppc64le.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1.0a0+gita8e7c98</t>
+    <t xml:space="preserve">2.1.0</t>
   </si>
   <si>
     <t xml:space="preserve">torch-2.1.0a0+gita8e7c98-cp39-cp39-linux_ppc64le.whl</t>
@@ -106,7 +109,7 @@
     <t xml:space="preserve">torchtext-0.16.2-cp39-cp39-linux_ppc64le.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">0.15.2a0+4571036</t>
+    <t xml:space="preserve">0.15.2</t>
   </si>
   <si>
     <t xml:space="preserve">torchtext-0.15.2a0+4571036-cp312-cp312-linux_ppc64le.whl</t>
@@ -130,15 +133,9 @@
     <t xml:space="preserve">torch-2.8.0-cp312-cp312-linux_ppc64le.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">0.15.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">torchtext-0.15.2-cp312-cp312-linux_ppc64le.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">torch-2.1.0-cp39-cp39-linux_ppc64le.whl</t>
   </si>
   <si>
@@ -433,13 +430,13 @@
     <t xml:space="preserve">vllm</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8.4+cpu</t>
+    <t xml:space="preserve">0.8.4</t>
   </si>
   <si>
     <t xml:space="preserve">vllm-0.8.4+cpu-cp312-cp312-linux_ppc64le.whl</t>
   </si>
   <si>
-    <t xml:space="preserve">0.10.0+cpu</t>
+    <t xml:space="preserve">0.10.0</t>
   </si>
   <si>
     <t xml:space="preserve">vllm-0.10.0+cpu-cp311-cp311-linux_ppc64le.whl</t>
@@ -461,6 +458,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -564,7 +562,20 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,10 +692,14 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.97"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -971,10 +986,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>3.12</v>
@@ -985,10 +1000,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>3.9</v>
@@ -996,13 +1011,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>3.11</v>
@@ -1010,13 +1025,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>3.12</v>
@@ -1024,13 +1039,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="4" t="n">
         <v>3.12</v>
@@ -1038,13 +1053,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>3.12</v>
@@ -1052,13 +1067,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>3.9</v>
@@ -1066,13 +1081,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>7</v>
@@ -1080,13 +1095,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>3.11</v>
@@ -1094,13 +1109,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>3.12</v>
@@ -1108,13 +1123,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>3.11</v>
@@ -1122,13 +1137,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>3.12</v>
@@ -1136,13 +1151,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>3.12</v>
@@ -1150,13 +1165,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="4" t="n">
         <v>3.12</v>
@@ -1164,13 +1179,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>7</v>
@@ -1178,13 +1193,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D36" s="4" t="n">
         <v>3.11</v>
@@ -1192,13 +1207,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D37" s="4" t="n">
         <v>3.11</v>
@@ -1206,13 +1221,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D38" s="4" t="n">
         <v>3.12</v>
@@ -1220,13 +1235,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>7</v>
@@ -1234,13 +1249,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>3.11</v>
@@ -1248,13 +1263,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D41" s="4" t="n">
         <v>3.12</v>
@@ -1262,13 +1277,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>7</v>
@@ -1276,13 +1291,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D43" s="4" t="n">
         <v>3.11</v>
@@ -1290,13 +1305,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>7</v>
@@ -1304,13 +1319,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>3.9</v>
@@ -1318,13 +1333,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>7</v>
@@ -1332,13 +1347,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>3.11</v>
@@ -1346,13 +1361,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>7</v>
@@ -1360,13 +1375,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>7</v>
@@ -1374,13 +1389,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D50" s="4" t="n">
         <v>3.11</v>
@@ -1388,13 +1403,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D51" s="4" t="n">
         <v>3.9</v>
@@ -1402,13 +1417,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>3.12</v>
@@ -1416,13 +1431,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>7</v>
@@ -1430,13 +1445,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>3.11</v>
@@ -1444,13 +1459,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>3.9</v>
@@ -1458,13 +1473,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>7</v>
@@ -1472,13 +1487,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D57" s="4" t="n">
         <v>3.11</v>
@@ -1486,13 +1501,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>3.12</v>
@@ -1500,13 +1515,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>3.13</v>
@@ -1514,13 +1529,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>7</v>
@@ -1528,13 +1543,13 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D61" s="4" t="n">
         <v>3.11</v>
@@ -1542,13 +1557,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>3.12</v>
@@ -1556,13 +1571,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>3.13</v>
@@ -1570,13 +1585,13 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>7</v>
@@ -1584,13 +1599,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>3.11</v>
@@ -1598,13 +1613,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D66" s="4" t="n">
         <v>3.12</v>
@@ -1612,13 +1627,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D67" s="4" t="n">
         <v>3.13</v>
@@ -1626,13 +1641,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
@@ -1640,13 +1655,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D69" s="4" t="n">
         <v>3.11</v>
@@ -1654,13 +1669,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D70" s="4" t="n">
         <v>3.12</v>
@@ -1668,13 +1683,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D71" s="4" t="n">
         <v>3.12</v>
@@ -1682,13 +1697,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>7</v>
@@ -1696,13 +1711,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D73" s="4" t="n">
         <v>3.11</v>
@@ -1710,13 +1725,13 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D74" s="4" t="n">
         <v>3.12</v>
@@ -1724,13 +1739,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D75" s="4" t="n">
         <v>3.13</v>
@@ -1738,13 +1753,13 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>7</v>
@@ -1752,13 +1767,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="D77" s="4" t="n">
         <v>3.11</v>
@@ -1766,13 +1781,13 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D78" s="4" t="n">
         <v>3.12</v>
@@ -1780,13 +1795,13 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D79" s="4" t="n">
         <v>3.13</v>
@@ -1794,13 +1809,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D80" s="4" t="n">
         <v>3.9</v>
@@ -1808,13 +1823,13 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D81" s="4" t="n">
         <v>3.9</v>
@@ -1822,13 +1837,13 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>7</v>
@@ -1836,13 +1851,13 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="D83" s="4" t="n">
         <v>3.11</v>
@@ -1850,13 +1865,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D84" s="4" t="n">
         <v>3.12</v>
@@ -1864,13 +1879,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D85" s="4" t="n">
         <v>3.13</v>
@@ -1878,13 +1893,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D86" s="4" t="n">
         <v>3.12</v>
@@ -1892,13 +1907,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D87" s="4" t="n">
         <v>3.12</v>
@@ -1906,13 +1921,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="D88" s="4" t="n">
         <v>3.12</v>
@@ -1920,13 +1935,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D89" s="4" t="n">
         <v>3.11</v>
@@ -1934,19 +1949,20 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D90" s="4" t="n">
         <v>3.12</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D90"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1954,5 +1970,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>